<commit_message>
Update RELATÓRIO DE DESFAZIMENTO DE BENS MÓVEIS PATRIMONIAIS DE 2021.xlsx
</commit_message>
<xml_diff>
--- a/testes_planilhas/RELATÓRIO DE DESFAZIMENTO DE BENS MÓVEIS PATRIMONIAIS DE 2021.xlsx
+++ b/testes_planilhas/RELATÓRIO DE DESFAZIMENTO DE BENS MÓVEIS PATRIMONIAIS DE 2021.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,158 @@
         </is>
       </c>
       <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>Alienação/Leilão</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>100111</v>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Quadro branco magnético 2.00m x 1.20m</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>01/08/2022</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>NF-e 49123</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>Coordenação do Curso de Pedagogia</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>Irrecuperável</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>Alienação/Leilão</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="1">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>100112</v>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Cadeira universitária com prancheta fixa</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>15/02/2020</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>NF-e 18990</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>Coordenação do Curso de História</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>Irrecuperável</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>Alienação/Leilão</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="30" customHeight="1">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>100113</v>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Longarina de 3 lugares para recepção, estofado azul</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>30/05/2019</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>NF-e 14321</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>Vice-Reitoria</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>Irrecuperável</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>Alienação/Leilão</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="30" customHeight="1">
+      <c r="A7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>100114</v>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Televisor Smart 50" 4K LG</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>05/04/2023</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>NF-e 53112</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>Pró-Reitoria de Graduação (PROGRAD)</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>Irrecuperável</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
         <is>
           <t>Alienação/Leilão</t>
         </is>

</xml_diff>